<commit_message>
13/12/2021 Minh updates LSTM in Reports folder
</commit_message>
<xml_diff>
--- a/Stocks/topcophieu.xlsx
+++ b/Stocks/topcophieu.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BACKUP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\PROJECT\CODE\stocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA74704C-D805-44AF-A794-9F4B40BA521D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBFE8235-9972-46C3-95DC-323ADE898B19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B80CB894-D490-43EC-9CE8-8E5889623959}"/>
+    <workbookView xWindow="2748" yWindow="3288" windowWidth="17280" windowHeight="9420" xr2:uid="{B80CB894-D490-43EC-9CE8-8E5889623959}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -273,9 +273,6 @@
     <t>DBC</t>
   </si>
   <si>
-    <t>PME</t>
-  </si>
-  <si>
     <t>CII</t>
   </si>
   <si>
@@ -327,9 +324,6 @@
     <t>HBC</t>
   </si>
   <si>
-    <t>VSH</t>
-  </si>
-  <si>
     <t>SZC</t>
   </si>
   <si>
@@ -946,15 +940,18 @@
   </si>
   <si>
     <t>VFS</t>
+  </si>
+  <si>
+    <t>HHS</t>
+  </si>
+  <si>
+    <t>PTL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="&quot;''&quot;@&quot;''&quot;"/>
-  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1024,7 +1021,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1341,23 +1338,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6DF112B-EA7C-46C0-8476-DA28150FF96B}">
   <dimension ref="A1:H101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E101"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="K64" sqref="K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D1" s="1"/>
       <c r="E1" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H1" s="2"/>
     </row>
@@ -1366,10 +1363,10 @@
         <v>18</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G2" s="3"/>
     </row>
@@ -1378,22 +1375,22 @@
         <v>53</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -1401,10 +1398,10 @@
         <v>20</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -1412,10 +1409,10 @@
         <v>40</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -1423,21 +1420,21 @@
         <v>5</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -1445,10 +1442,10 @@
         <v>23</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1456,32 +1453,32 @@
         <v>76</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1489,10 +1486,10 @@
         <v>7</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
@@ -1500,10 +1497,10 @@
         <v>77</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -1511,10 +1508,10 @@
         <v>60</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
@@ -1522,32 +1519,32 @@
         <v>51</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1555,10 +1552,10 @@
         <v>44</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1566,10 +1563,10 @@
         <v>56</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1577,10 +1574,10 @@
         <v>64</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1588,10 +1585,10 @@
         <v>48</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,21 +1596,21 @@
         <v>32</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1621,10 +1618,10 @@
         <v>21</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1632,21 +1629,21 @@
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1654,10 +1651,10 @@
         <v>49</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1665,10 +1662,10 @@
         <v>54</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1676,10 +1673,10 @@
         <v>70</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,32 +1684,32 @@
         <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1720,10 +1717,10 @@
         <v>55</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1731,10 +1728,10 @@
         <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1742,329 +1739,329 @@
         <v>67</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="4" t="s">
-        <v>45</v>
+        <v>301</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="4" t="s">
-        <v>57</v>
+        <v>6</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="4" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
-        <v>24</v>
+        <v>68</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="4" t="s">
-        <v>71</v>
+        <v>24</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="4" t="s">
-        <v>93</v>
+        <v>71</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="4" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="4" t="s">
-        <v>36</v>
+        <v>73</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="4" t="s">
-        <v>37</v>
+        <v>47</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="4" t="s">
-        <v>98</v>
+        <v>37</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="4" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="4" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
-        <v>15</v>
+        <v>39</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="4" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="4" t="s">
-        <v>11</v>
+        <v>31</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="4" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="4" t="s">
-        <v>52</v>
+        <v>19</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
-        <v>69</v>
+        <v>52</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="4" t="s">
-        <v>13</v>
+        <v>69</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="4" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="4" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="4" t="s">
-        <v>29</v>
+        <v>82</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
-        <v>61</v>
+        <v>29</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="4" t="s">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="4" t="s">
-        <v>78</v>
+        <v>17</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2072,21 +2069,21 @@
         <v>35</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2094,10 +2091,10 @@
         <v>27</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2105,362 +2102,362 @@
         <v>58</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="4" t="s">
-        <v>50</v>
+        <v>302</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="4" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="4" t="s">
-        <v>38</v>
+        <v>74</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="4" t="s">
-        <v>10</v>
+        <v>38</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="4" t="s">
-        <v>99</v>
+        <v>10</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="4" t="s">
-        <v>42</v>
+        <v>97</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="4" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="4" t="s">
-        <v>33</v>
+        <v>90</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="4" t="s">
-        <v>97</v>
+        <v>26</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="4" t="s">
-        <v>8</v>
+        <v>95</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="4" t="s">
-        <v>62</v>
+        <v>8</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="4" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="4" t="s">
-        <v>28</v>
+        <v>85</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E84" s="4" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="4" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="E85" s="4" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="4" t="s">
-        <v>72</v>
+        <v>1</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="4" t="s">
-        <v>34</v>
+        <v>72</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="4" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="4" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="4" t="s">
-        <v>63</v>
+        <v>41</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="4" t="s">
-        <v>2</v>
+        <v>63</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="4" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="4" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="E93" s="4" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="4" t="s">
-        <v>84</v>
+        <v>0</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="E94" s="4" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="4" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E95" s="4" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="4" t="s">
-        <v>75</v>
+        <v>16</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="E96" s="4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="4" t="s">
-        <v>3</v>
+        <v>75</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="4" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="4" t="s">
-        <v>65</v>
+        <v>12</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E99" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="4" t="s">
-        <v>14</v>
+        <v>65</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
-        <v>96</v>
+        <v>14</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
   </sheetData>

</xml_diff>